<commit_message>
added more risk drivers and their text and changed overwrite
</commit_message>
<xml_diff>
--- a/Expert_weights.xlsx
+++ b/Expert_weights.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IrisReitsmaRiskQuest\Projects\Circular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IrisReitsmaRiskQuest\Documents\GitHub\dasbhoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD610EF7-D3F4-404E-9111-3E0AAEFB19F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6784DC-200E-4002-B35F-B3752F217C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B959621-CE8C-40AE-BCFC-16B25DBD14E7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Ability of Management Team</t>
   </si>
@@ -44,48 +44,15 @@
     <t>Suitability of product for Circularity</t>
   </si>
   <si>
-    <t>Technology &amp; business model maturity</t>
-  </si>
-  <si>
-    <t>Resource availability</t>
-  </si>
-  <si>
     <t>Circularity of asset</t>
   </si>
   <si>
-    <t>Customer revenue retention</t>
-  </si>
-  <si>
     <t>Market competitiveness</t>
   </si>
   <si>
     <t>Robustness of contract</t>
   </si>
   <si>
-    <t>Liquidity</t>
-  </si>
-  <si>
-    <t>Key supplier(s) relationship(s) / dependency risk</t>
-  </si>
-  <si>
-    <t>Compliance to sustainability policies</t>
-  </si>
-  <si>
-    <t>Customer concentration</t>
-  </si>
-  <si>
-    <t>Operator dependency</t>
-  </si>
-  <si>
-    <t>Financed entity</t>
-  </si>
-  <si>
-    <t>Company size</t>
-  </si>
-  <si>
-    <t>Circularity of the balance sheet</t>
-  </si>
-  <si>
     <t>Risk Factor</t>
   </si>
   <si>
@@ -102,6 +69,9 @@
   </si>
   <si>
     <t>Total avg score</t>
+  </si>
+  <si>
+    <t>Security of resources</t>
   </si>
 </sst>
 </file>
@@ -461,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E351150B-9EA8-464C-87A9-8765234B11B5}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -479,22 +449,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -539,282 +509,82 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="C4">
-        <v>10.027272727272727</v>
+        <v>11.818181818181818</v>
       </c>
       <c r="D4">
-        <v>10.25</v>
+        <v>4.25</v>
       </c>
       <c r="E4">
-        <v>9.6</v>
+        <v>6.2</v>
       </c>
       <c r="F4">
-        <v>7.9280303030303036</v>
+        <v>7.8409090909090908</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>3.6666666666666665</v>
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>11.818181818181818</v>
+        <v>7.5545454545454547</v>
       </c>
       <c r="D5">
-        <v>4.25</v>
+        <v>12.5</v>
       </c>
       <c r="E5">
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="F5">
-        <v>7.8409090909090908</v>
+        <v>7.7727272727272725</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D6">
+        <v>6.25</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="F6">
         <v>5</v>
-      </c>
-      <c r="C6">
-        <v>7.5545454545454547</v>
-      </c>
-      <c r="D6">
-        <v>12.5</v>
-      </c>
-      <c r="E6">
-        <v>7.8</v>
-      </c>
-      <c r="F6">
-        <v>7.7727272727272725</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>8.3333333333333339</v>
+        <v>13.666666666666666</v>
       </c>
       <c r="C7">
-        <v>4.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D7">
-        <v>8.5</v>
+        <v>4.75</v>
       </c>
       <c r="E7">
-        <v>13.6</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>6.875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D8">
-        <v>6.25</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>13.666666666666666</v>
-      </c>
-      <c r="C9">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D9">
-        <v>4.75</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
         <v>4.833333333333333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>10.666666666666666</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>7.5</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <v>4.791666666666667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="C11">
-        <v>5.8090909090909095</v>
-      </c>
-      <c r="D11">
-        <v>4.25</v>
-      </c>
-      <c r="E11">
-        <v>3.8</v>
-      </c>
-      <c r="F11">
-        <v>3.9621212121212124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="C12">
-        <v>5.2</v>
-      </c>
-      <c r="D12">
-        <v>1.5</v>
-      </c>
-      <c r="E12">
-        <v>1.8</v>
-      </c>
-      <c r="F12">
-        <v>2.5833333333333335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>1.6</v>
-      </c>
-      <c r="D13">
-        <v>6.5</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>2.5416666666666665</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>3.2</v>
-      </c>
-      <c r="D14">
-        <v>1.5</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>2.2916666666666665</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>1.5</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>2.1666666666666665</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>1.7</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16">
-        <v>2.125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="C17">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D17">
-        <v>2.75</v>
-      </c>
-      <c r="E17">
-        <v>0.8</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small weights bug fix
</commit_message>
<xml_diff>
--- a/Expert_weights.xlsx
+++ b/Expert_weights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IrisReitsmaRiskQuest\Documents\GitHub\dasbhoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6784DC-200E-4002-B35F-B3752F217C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0BC90-15CF-4637-A706-096293552303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B959621-CE8C-40AE-BCFC-16B25DBD14E7}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -589,5 +589,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added all risk drivers and examples, a feedback form and input is correctly stored
</commit_message>
<xml_diff>
--- a/Expert_weights.xlsx
+++ b/Expert_weights.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IrisReitsmaRiskQuest\Documents\GitHub\dasbhoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0BC90-15CF-4637-A706-096293552303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9EEE08-F980-4E1B-979C-70301C76C754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7B959621-CE8C-40AE-BCFC-16B25DBD14E7}"/>
   </bookViews>

</xml_diff>